<commit_message>
lots of data organization
</commit_message>
<xml_diff>
--- a/Data/columns.xlsx
+++ b/Data/columns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeldaraptor\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\rbarmstrong\co2seq\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A835488A-89A2-4930-B3C7-5E2D7482BC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62DE311-42A6-402C-B9ED-4D5299932BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{23BDBD4F-21E0-334D-9395-516C3763FCFF}"/>
+    <workbookView xWindow="-5520" yWindow="1140" windowWidth="17280" windowHeight="8964" xr2:uid="{23BDBD4F-21E0-334D-9395-516C3763FCFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -853,7 +853,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -862,27 +862,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Unicode MS"/>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -890,30 +886,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1230,1535 +1209,1439 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B570C022-9258-454E-AB6C-EF28F1F278B9}">
   <dimension ref="A1:B283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.796875" customWidth="1"/>
+    <col min="2" max="2" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>37</v>
       </c>
       <c r="B42" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>38</v>
       </c>
       <c r="B48" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="2" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>65</v>
       </c>
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="2" t="s">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>66</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="2" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>67</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="2" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>68</v>
       </c>
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="2" t="s">
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>69</v>
       </c>
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="2" t="s">
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>70</v>
       </c>
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="2" t="s">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>71</v>
       </c>
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="2" t="s">
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>72</v>
       </c>
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="2" t="s">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>73</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="2" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>74</v>
       </c>
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="2" t="s">
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>75</v>
       </c>
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="2" t="s">
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>76</v>
       </c>
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="2" t="s">
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>77</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="2" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>78</v>
       </c>
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="2" t="s">
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>79</v>
       </c>
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="2" t="s">
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>80</v>
       </c>
-      <c r="B94" s="3"/>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="2" t="s">
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>81</v>
       </c>
-      <c r="B95" s="3"/>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="2" t="s">
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>82</v>
       </c>
-      <c r="B96" s="3"/>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="2" t="s">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>83</v>
       </c>
-      <c r="B97" s="3"/>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="2" t="s">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>84</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B98" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="2" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>85</v>
       </c>
-      <c r="B99" s="3"/>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="2" t="s">
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>86</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="2" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>87</v>
       </c>
-      <c r="B101" s="3"/>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="2" t="s">
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>88</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B102" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="2" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>89</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B103" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="2" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>90</v>
       </c>
-      <c r="B104" s="3"/>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="2" t="s">
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>91</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B105" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="2" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>92</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="2" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>93</v>
       </c>
-      <c r="B107" s="3"/>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="2" t="s">
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>94</v>
       </c>
-      <c r="B108" s="3"/>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="2" t="s">
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>95</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="2" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>96</v>
       </c>
-      <c r="B110" s="3"/>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="2" t="s">
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>97</v>
       </c>
-      <c r="B111" s="3"/>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="2" t="s">
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>98</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="2" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>99</v>
       </c>
-      <c r="B113" s="3"/>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="2" t="s">
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>100</v>
       </c>
-      <c r="B114" s="3"/>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="A115" s="2" t="s">
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>101</v>
       </c>
-      <c r="B115" s="3"/>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="A116" s="2" t="s">
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>102</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B116" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="2" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>103</v>
       </c>
-      <c r="B117" s="3"/>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="2" t="s">
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>104</v>
       </c>
-      <c r="B118" s="3"/>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="2" t="s">
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>105</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B119" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
-      <c r="A120" s="2" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>106</v>
       </c>
-      <c r="B120" s="3"/>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" s="2" t="s">
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
         <v>107</v>
       </c>
-      <c r="B121" s="3"/>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="A122" s="2" t="s">
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
         <v>108</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B122" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
-      <c r="A123" s="2" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
         <v>109</v>
       </c>
-      <c r="B123" s="3"/>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="A124" s="2" t="s">
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
         <v>110</v>
       </c>
-      <c r="B124" s="3"/>
-    </row>
-    <row r="125" spans="1:2">
-      <c r="A125" s="2" t="s">
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>111</v>
       </c>
-      <c r="B125" s="3"/>
-    </row>
-    <row r="126" spans="1:2">
-      <c r="A126" s="2" t="s">
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>112</v>
       </c>
-      <c r="B126" s="3" t="s">
+      <c r="B126" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
-      <c r="A127" s="2" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>113</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B127" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
-      <c r="A128" s="2" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
         <v>114</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B128" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
-      <c r="A129" s="2" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>115</v>
       </c>
-      <c r="B129" s="3" t="s">
+      <c r="B129" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
-      <c r="A130" s="2" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>116</v>
       </c>
-      <c r="B130" s="3"/>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="A131" s="2" t="s">
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>117</v>
       </c>
-      <c r="B131" s="3"/>
-    </row>
-    <row r="132" spans="1:2">
-      <c r="A132" s="2" t="s">
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>118</v>
       </c>
-      <c r="B132" s="3"/>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133" s="2" t="s">
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
         <v>119</v>
       </c>
-      <c r="B133" s="3"/>
-    </row>
-    <row r="134" spans="1:2">
-      <c r="A134" s="2" t="s">
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
         <v>120</v>
       </c>
-      <c r="B134" s="3"/>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135" s="2" t="s">
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
         <v>121</v>
       </c>
-      <c r="B135" s="3"/>
-    </row>
-    <row r="136" spans="1:2">
-      <c r="A136" s="2" t="s">
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
         <v>122</v>
       </c>
-      <c r="B136" s="3"/>
-    </row>
-    <row r="137" spans="1:2">
-      <c r="A137" s="2" t="s">
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>123</v>
       </c>
-      <c r="B137" s="3" t="s">
+      <c r="B137" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
-      <c r="A138" s="2" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
         <v>124</v>
       </c>
-      <c r="B138" s="3"/>
-    </row>
-    <row r="139" spans="1:2">
-      <c r="A139" s="2" t="s">
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>125</v>
       </c>
-      <c r="B139" s="3" t="s">
+      <c r="B139" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
-      <c r="A140" s="2" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
         <v>126</v>
       </c>
-      <c r="B140" s="3"/>
-    </row>
-    <row r="141" spans="1:2">
-      <c r="A141" s="2" t="s">
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
         <v>127</v>
       </c>
-      <c r="B141" s="3"/>
-    </row>
-    <row r="142" spans="1:2">
-      <c r="A142" s="2" t="s">
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
         <v>128</v>
       </c>
-      <c r="B142" s="3"/>
-    </row>
-    <row r="143" spans="1:2">
-      <c r="A143" s="2" t="s">
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
         <v>129</v>
       </c>
-      <c r="B143" s="3"/>
-    </row>
-    <row r="144" spans="1:2">
-      <c r="A144" s="2" t="s">
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
         <v>130</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B144" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
-      <c r="A145" s="2" t="s">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
         <v>131</v>
       </c>
-      <c r="B145" s="3"/>
-    </row>
-    <row r="146" spans="1:2">
-      <c r="A146" s="2" t="s">
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>132</v>
       </c>
-      <c r="B146" s="3"/>
-    </row>
-    <row r="147" spans="1:2">
-      <c r="A147" s="2" t="s">
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
         <v>133</v>
       </c>
-      <c r="B147" s="3"/>
-    </row>
-    <row r="148" spans="1:2">
-      <c r="A148" s="2" t="s">
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
         <v>134</v>
       </c>
-      <c r="B148" s="3"/>
-    </row>
-    <row r="149" spans="1:2">
-      <c r="A149" s="2" t="s">
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
         <v>135</v>
       </c>
-      <c r="B149" s="3"/>
-    </row>
-    <row r="150" spans="1:2">
-      <c r="A150" s="2" t="s">
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
         <v>136</v>
       </c>
-      <c r="B150" s="3"/>
-    </row>
-    <row r="151" spans="1:2">
-      <c r="A151" s="2" t="s">
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
         <v>137</v>
       </c>
-      <c r="B151" s="3"/>
-    </row>
-    <row r="152" spans="1:2">
-      <c r="A152" s="2" t="s">
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
         <v>138</v>
       </c>
-      <c r="B152" s="3"/>
-    </row>
-    <row r="153" spans="1:2">
-      <c r="A153" s="2" t="s">
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
         <v>139</v>
       </c>
-      <c r="B153" s="3"/>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154" s="2" t="s">
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
         <v>140</v>
       </c>
-      <c r="B154" s="3"/>
-    </row>
-    <row r="155" spans="1:2">
-      <c r="A155" s="2" t="s">
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
         <v>141</v>
       </c>
-      <c r="B155" s="3"/>
-    </row>
-    <row r="156" spans="1:2">
-      <c r="A156" s="2" t="s">
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
         <v>142</v>
       </c>
-      <c r="B156" s="3"/>
-    </row>
-    <row r="157" spans="1:2">
-      <c r="A157" s="2" t="s">
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
         <v>143</v>
       </c>
-      <c r="B157" s="3"/>
-    </row>
-    <row r="158" spans="1:2">
-      <c r="A158" s="2" t="s">
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
         <v>144</v>
       </c>
-      <c r="B158" s="3"/>
-    </row>
-    <row r="159" spans="1:2">
-      <c r="A159" s="2" t="s">
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
         <v>57</v>
       </c>
-      <c r="B159" s="3"/>
-    </row>
-    <row r="160" spans="1:2">
-      <c r="A160" s="2" t="s">
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
         <v>145</v>
       </c>
-      <c r="B160" s="3"/>
-    </row>
-    <row r="161" spans="1:2">
-      <c r="A161" s="2" t="s">
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
         <v>32</v>
       </c>
-      <c r="B161" s="3"/>
-    </row>
-    <row r="163" spans="1:2">
-      <c r="A163" s="1" t="s">
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
-      <c r="A165" s="1" t="s">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
         <v>147</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
-      <c r="A166" s="1" t="s">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
         <v>148</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
-      <c r="A167" s="1" t="s">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
-      <c r="A168" s="1" t="s">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
-      <c r="A169" s="1" t="s">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
-      <c r="A170" s="1" t="s">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
-      <c r="A172" s="1" t="s">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
-      <c r="A174" s="1" t="s">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
-      <c r="A175" s="1" t="s">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
-      <c r="A176" s="1" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
-      <c r="A177" s="1" t="s">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
-      <c r="A178" s="1" t="s">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
-      <c r="A179" s="1" t="s">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
-      <c r="A181" s="1" t="s">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
         <v>156</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
-      <c r="A183" s="1" t="s">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
-      <c r="A184" s="1" t="s">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
-      <c r="A185" s="1" t="s">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
-      <c r="A186" s="1" t="s">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
         <v>160</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B186" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
-      <c r="A187" s="1" t="s">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
-      <c r="A188" s="1" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
-      <c r="A189" s="1" t="s">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
-      <c r="A190" s="1" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
-      <c r="A191" s="1" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
-      <c r="A193" s="1" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
-      <c r="A195" s="1" t="s">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
-      <c r="A196" s="1" t="s">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
-      <c r="A197" s="1" t="s">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
-      <c r="A198" s="1" t="s">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
-      <c r="A200" s="1" t="s">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
-      <c r="A202" s="1" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
         <v>170</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B202" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
-      <c r="A203" s="1" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
-      <c r="A204" s="1" t="s">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
-      <c r="A205" s="1" t="s">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
-      <c r="A206" s="1" t="s">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
-      <c r="A208" s="1" t="s">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="210" spans="1:1">
-      <c r="A210" s="1" t="s">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="211" spans="1:1">
-      <c r="A211" s="1" t="s">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="212" spans="1:1">
-      <c r="A212" s="1" t="s">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="213" spans="1:1">
-      <c r="A213" s="1" t="s">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="215" spans="1:1">
-      <c r="A215" s="1" t="s">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="217" spans="1:1">
-      <c r="A217" s="1" t="s">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="218" spans="1:1">
-      <c r="A218" s="1" t="s">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="219" spans="1:1">
-      <c r="A219" s="1" t="s">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="220" spans="1:1">
-      <c r="A220" s="1" t="s">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="222" spans="1:1">
-      <c r="A222" s="1" t="s">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="224" spans="1:1">
-      <c r="A224" s="1" t="s">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
-      <c r="A225" s="1" t="s">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
-      <c r="A226" s="1" t="s">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
         <v>178</v>
       </c>
       <c r="B226" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
-      <c r="A227" s="1" t="s">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
-      <c r="A228" s="1" t="s">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
-      <c r="A229" s="1" t="s">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
-      <c r="A230" s="1" t="s">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
-      <c r="A231" s="1" t="s">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
-      <c r="A232" s="1" t="s">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
-      <c r="A234" s="2" t="s">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
         <v>184</v>
       </c>
-      <c r="B234" s="3"/>
-    </row>
-    <row r="235" spans="1:2">
-      <c r="A235" s="3"/>
-      <c r="B235" s="3"/>
-    </row>
-    <row r="236" spans="1:2">
-      <c r="A236" s="2" t="s">
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
         <v>185</v>
       </c>
-      <c r="B236" s="3"/>
-    </row>
-    <row r="237" spans="1:2">
-      <c r="A237" s="2" t="s">
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
         <v>186</v>
       </c>
-      <c r="B237" s="3"/>
-    </row>
-    <row r="238" spans="1:2">
-      <c r="A238" s="2" t="s">
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
         <v>187</v>
       </c>
-      <c r="B238" s="3"/>
-    </row>
-    <row r="239" spans="1:2">
-      <c r="A239" s="2" t="s">
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
         <v>188</v>
       </c>
-      <c r="B239" s="3"/>
-    </row>
-    <row r="240" spans="1:2">
-      <c r="A240" s="2" t="s">
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
         <v>189</v>
       </c>
-      <c r="B240" s="3"/>
-    </row>
-    <row r="241" spans="1:2">
-      <c r="A241" s="2" t="s">
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
         <v>190</v>
       </c>
-      <c r="B241" s="3" t="s">
+      <c r="B241" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
-      <c r="A242" s="2" t="s">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
         <v>191</v>
       </c>
-      <c r="B242" s="3"/>
-    </row>
-    <row r="243" spans="1:2">
-      <c r="A243" s="2" t="s">
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
         <v>192</v>
       </c>
-      <c r="B243" s="3"/>
-    </row>
-    <row r="244" spans="1:2">
-      <c r="A244" s="2" t="s">
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
         <v>193</v>
       </c>
-      <c r="B244" s="3" t="s">
+      <c r="B244" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
-      <c r="A245" s="2" t="s">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
         <v>194</v>
       </c>
-      <c r="B245" s="3" t="s">
+      <c r="B245" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
-      <c r="A246" s="2" t="s">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
         <v>195</v>
       </c>
-      <c r="B246" s="3"/>
-    </row>
-    <row r="247" spans="1:2">
-      <c r="A247" s="2" t="s">
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
         <v>196</v>
       </c>
-      <c r="B247" s="3"/>
-    </row>
-    <row r="248" spans="1:2">
-      <c r="A248" s="2" t="s">
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
         <v>197</v>
       </c>
-      <c r="B248" s="3"/>
-    </row>
-    <row r="249" spans="1:2">
-      <c r="A249" s="2" t="s">
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
         <v>198</v>
       </c>
-      <c r="B249" s="3"/>
-    </row>
-    <row r="250" spans="1:2">
-      <c r="A250" s="2" t="s">
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
         <v>199</v>
       </c>
-      <c r="B250" s="3"/>
-    </row>
-    <row r="251" spans="1:2">
-      <c r="A251" s="2" t="s">
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
         <v>200</v>
       </c>
-      <c r="B251" s="3"/>
-    </row>
-    <row r="252" spans="1:2">
-      <c r="A252" s="2" t="s">
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
         <v>201</v>
       </c>
-      <c r="B252" s="3"/>
-    </row>
-    <row r="253" spans="1:2">
-      <c r="A253" s="2" t="s">
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
         <v>202</v>
       </c>
-      <c r="B253" s="3"/>
-    </row>
-    <row r="254" spans="1:2">
-      <c r="A254" s="2" t="s">
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
         <v>203</v>
       </c>
-      <c r="B254" s="3"/>
-    </row>
-    <row r="255" spans="1:2">
-      <c r="A255" s="2" t="s">
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
         <v>204</v>
       </c>
-      <c r="B255" s="3"/>
-    </row>
-    <row r="256" spans="1:2">
-      <c r="A256" s="2" t="s">
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
         <v>205</v>
       </c>
-      <c r="B256" s="3"/>
-    </row>
-    <row r="257" spans="1:2">
-      <c r="A257" s="2" t="s">
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
         <v>206</v>
       </c>
-      <c r="B257" s="3"/>
-    </row>
-    <row r="258" spans="1:2">
-      <c r="A258" s="2" t="s">
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
         <v>207</v>
       </c>
-      <c r="B258" s="3" t="s">
+      <c r="B258" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
-      <c r="A259" s="2" t="s">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
         <v>208</v>
       </c>
-      <c r="B259" s="3"/>
-    </row>
-    <row r="260" spans="1:2">
-      <c r="A260" s="2" t="s">
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
         <v>209</v>
       </c>
-      <c r="B260" s="3" t="s">
+      <c r="B260" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
-      <c r="A261" s="2" t="s">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
         <v>210</v>
       </c>
-      <c r="B261" s="3"/>
-    </row>
-    <row r="262" spans="1:2">
-      <c r="A262" s="2" t="s">
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
         <v>211</v>
       </c>
-      <c r="B262" s="3"/>
-    </row>
-    <row r="263" spans="1:2">
-      <c r="A263" s="2" t="s">
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
         <v>212</v>
       </c>
-      <c r="B263" s="3" t="s">
+      <c r="B263" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
-      <c r="A264" s="2" t="s">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
         <v>213</v>
       </c>
-      <c r="B264" s="3" t="s">
+      <c r="B264" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
-      <c r="A265" s="2" t="s">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
         <v>214</v>
       </c>
-      <c r="B265" s="3" t="s">
+      <c r="B265" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
-      <c r="A266" s="2" t="s">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
         <v>215</v>
       </c>
-      <c r="B266" s="3" t="s">
+      <c r="B266" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
-      <c r="A267" s="2" t="s">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
         <v>216</v>
       </c>
-      <c r="B267" s="3"/>
-    </row>
-    <row r="268" spans="1:2">
-      <c r="A268" s="2" t="s">
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
         <v>217</v>
       </c>
-      <c r="B268" s="3"/>
-    </row>
-    <row r="269" spans="1:2">
-      <c r="A269" s="2" t="s">
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
         <v>218</v>
       </c>
-      <c r="B269" s="3"/>
-    </row>
-    <row r="270" spans="1:2">
-      <c r="A270" s="2" t="s">
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
         <v>219</v>
       </c>
-      <c r="B270" s="3" t="s">
+      <c r="B270" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
-      <c r="A271" s="2" t="s">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
         <v>220</v>
       </c>
-      <c r="B271" s="3"/>
-    </row>
-    <row r="272" spans="1:2">
-      <c r="A272" s="2" t="s">
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
         <v>32</v>
       </c>
-      <c r="B272" s="3"/>
-    </row>
-    <row r="274" spans="1:2">
-      <c r="A274" s="1" t="s">
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="276" spans="1:2">
-      <c r="A276" s="1" t="s">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
-      <c r="A277" s="1" t="s">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
-      <c r="A278" s="1" t="s">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
-      <c r="A279" s="1" t="s">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
-      <c r="A280" s="1" t="s">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
         <v>225</v>
       </c>
       <c r="B280" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
-      <c r="A281" s="1" t="s">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
-      <c r="A282" s="1" t="s">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
-      <c r="A283" s="1" t="s">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>